<commit_message>
mudei muita coisa, tentei deixar mais organizado e modularizado as operacoes com as issues
</commit_message>
<xml_diff>
--- a/Issues por Sprint.xlsx
+++ b/Issues por Sprint.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://tcucloud-my.sharepoint.com/personal/x13802311752_tcu_gov_br/Documents/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Henrique Givisiez\.vscode\Python\Github Issues Automation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{11DE42F9-62F4-40AB-BBEF-09326DBF8ECB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87E22882-C8B3-4CAE-9C2F-F886B1FA55BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{555AA5F7-C304-4351-8848-CF7D37BD15A5}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{555AA5F7-C304-4351-8848-CF7D37BD15A5}"/>
   </bookViews>
   <sheets>
     <sheet name="Sprint2" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="38">
   <si>
     <t>Etapa</t>
   </si>
@@ -144,16 +144,28 @@
   </si>
   <si>
     <t>Exibir toast de confirmação que o garçom foi chamado</t>
+  </si>
+  <si>
+    <t>Sprint</t>
+  </si>
+  <si>
+    <t>Sprint 2</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -521,10 +533,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{731DB60A-8110-489D-97EC-342F9C438071}">
-  <dimension ref="A1:C25"/>
+  <dimension ref="A1:D25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+      <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -534,7 +546,7 @@
     <col min="3" max="3" width="7.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -544,8 +556,11 @@
       <c r="C1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="D1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
@@ -555,8 +570,11 @@
       <c r="C2" s="1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D2" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>6</v>
       </c>
@@ -566,8 +584,11 @@
       <c r="C3" s="1" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D3" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>9</v>
       </c>
@@ -577,8 +598,11 @@
       <c r="C4" s="1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D4" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>11</v>
       </c>
@@ -588,8 +612,11 @@
       <c r="C5" s="1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D5" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>11</v>
       </c>
@@ -599,8 +626,11 @@
       <c r="C6" s="1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="D6" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>14</v>
       </c>
@@ -610,8 +640,11 @@
       <c r="C7" s="1" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D7" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>16</v>
       </c>
@@ -621,8 +654,11 @@
       <c r="C8" s="1" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D8" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>11</v>
       </c>
@@ -632,8 +668,11 @@
       <c r="C9" s="1" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D9" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>11</v>
       </c>
@@ -643,8 +682,11 @@
       <c r="C10" s="2" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="11" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="D10" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>11</v>
       </c>
@@ -654,8 +696,11 @@
       <c r="C11" s="2" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D11" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>11</v>
       </c>
@@ -665,8 +710,11 @@
       <c r="C12" s="2" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="13" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="D12" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>11</v>
       </c>
@@ -676,8 +724,11 @@
       <c r="C13" s="2" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="14" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="D13" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>3</v>
       </c>
@@ -687,8 +738,11 @@
       <c r="C14" s="2" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D14" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>11</v>
       </c>
@@ -698,8 +752,11 @@
       <c r="C15" s="2" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D15" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>11</v>
       </c>
@@ -709,8 +766,11 @@
       <c r="C16" s="2" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D16" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
         <v>11</v>
       </c>
@@ -720,8 +780,11 @@
       <c r="C17" s="2" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="18" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="D17" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
         <v>11</v>
       </c>
@@ -731,8 +794,11 @@
       <c r="C18" s="2" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D18" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
         <v>9</v>
       </c>
@@ -742,8 +808,11 @@
       <c r="C19" s="2" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="20" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="D19" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
         <v>11</v>
       </c>
@@ -753,8 +822,11 @@
       <c r="C20" s="2" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D20" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
         <v>16</v>
       </c>
@@ -764,8 +836,11 @@
       <c r="C21" s="2" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D21" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
         <v>11</v>
       </c>
@@ -775,8 +850,11 @@
       <c r="C22" s="2" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="23" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="D22" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
         <v>6</v>
       </c>
@@ -786,8 +864,11 @@
       <c r="C23" s="2" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D23" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
         <v>9</v>
       </c>
@@ -797,8 +878,11 @@
       <c r="C24" s="2" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D24" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
         <v>11</v>
       </c>
@@ -808,8 +892,12 @@
       <c r="C25" s="2" t="s">
         <v>8</v>
       </c>
+      <c r="D25" s="1" t="s">
+        <v>37</v>
+      </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>
 </file>
</xml_diff>